<commit_message>
last commit before release.2
</commit_message>
<xml_diff>
--- a/src/test/resources/DataDriven/TestData.xlsx
+++ b/src/test/resources/DataDriven/TestData.xlsx
@@ -374,10 +374,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D1:D2"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -385,13 +385,13 @@
     <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D1" s="1" t="s">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D2" t="s">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>